<commit_message>
Another fix for the minor fix
</commit_message>
<xml_diff>
--- a/SocioSpatial Experiment MatlabCode/corpus/ActualMaster.xlsx
+++ b/SocioSpatial Experiment MatlabCode/corpus/ActualMaster.xlsx
@@ -2499,10 +2499,10 @@
         <v>262</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>286</v>
@@ -2951,7 +2951,7 @@
         <v>285</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>294</v>
@@ -3013,7 +3013,7 @@
         <v>285</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>294</v>
@@ -3447,7 +3447,7 @@
         <v>285</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>305</v>
@@ -3509,7 +3509,7 @@
         <v>285</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>305</v>
@@ -3943,7 +3943,7 @@
         <v>285</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>316</v>
@@ -4005,7 +4005,7 @@
         <v>285</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>316</v>
@@ -4439,7 +4439,7 @@
         <v>285</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>330</v>
+        <v>285</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>326</v>
@@ -4501,7 +4501,7 @@
         <v>285</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>285</v>
+        <v>330</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>326</v>
@@ -4935,7 +4935,7 @@
         <v>285</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>341</v>
+        <v>285</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>337</v>
@@ -4997,7 +4997,7 @@
         <v>285</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>285</v>
+        <v>341</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>337</v>
@@ -5431,7 +5431,7 @@
         <v>285</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>348</v>
@@ -5493,7 +5493,7 @@
         <v>285</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>348</v>
@@ -5927,7 +5927,7 @@
         <v>285</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>366</v>
+        <v>285</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>362</v>
@@ -5989,7 +5989,7 @@
         <v>285</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>285</v>
+        <v>366</v>
       </c>
       <c r="K65" s="4" t="s">
         <v>362</v>
@@ -6423,7 +6423,7 @@
         <v>285</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>376</v>
+        <v>285</v>
       </c>
       <c r="K72" s="4" t="s">
         <v>372</v>
@@ -6485,7 +6485,7 @@
         <v>285</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>285</v>
+        <v>376</v>
       </c>
       <c r="K73" s="4" t="s">
         <v>372</v>
@@ -6919,7 +6919,7 @@
         <v>285</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>386</v>
+        <v>285</v>
       </c>
       <c r="K80" s="4" t="s">
         <v>381</v>
@@ -6981,7 +6981,7 @@
         <v>285</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>285</v>
+        <v>386</v>
       </c>
       <c r="K81" s="4" t="s">
         <v>381</v>
@@ -7415,7 +7415,7 @@
         <v>285</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>400</v>
+        <v>285</v>
       </c>
       <c r="K88" s="4" t="s">
         <v>391</v>
@@ -7477,7 +7477,7 @@
         <v>285</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>285</v>
+        <v>400</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>391</v>
@@ -7911,7 +7911,7 @@
         <v>285</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>406</v>
+        <v>285</v>
       </c>
       <c r="K96" s="4" t="s">
         <v>402</v>
@@ -7973,7 +7973,7 @@
         <v>285</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>285</v>
+        <v>406</v>
       </c>
       <c r="K97" s="4" t="s">
         <v>402</v>
@@ -8407,7 +8407,7 @@
         <v>285</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>416</v>
+        <v>285</v>
       </c>
       <c r="K104" s="4" t="s">
         <v>412</v>
@@ -8469,7 +8469,7 @@
         <v>285</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>285</v>
+        <v>416</v>
       </c>
       <c r="K105" s="4" t="s">
         <v>412</v>
@@ -8903,7 +8903,7 @@
         <v>285</v>
       </c>
       <c r="J112" s="4" t="s">
-        <v>431</v>
+        <v>285</v>
       </c>
       <c r="K112" s="4" t="s">
         <v>422</v>
@@ -8965,7 +8965,7 @@
         <v>285</v>
       </c>
       <c r="J113" s="4" t="s">
-        <v>285</v>
+        <v>431</v>
       </c>
       <c r="K113" s="4" t="s">
         <v>422</v>
@@ -9399,7 +9399,7 @@
         <v>285</v>
       </c>
       <c r="J120" s="4" t="s">
-        <v>437</v>
+        <v>285</v>
       </c>
       <c r="K120" s="4" t="s">
         <v>433</v>
@@ -9461,7 +9461,7 @@
         <v>285</v>
       </c>
       <c r="J121" s="4" t="s">
-        <v>285</v>
+        <v>437</v>
       </c>
       <c r="K121" s="4" t="s">
         <v>433</v>
@@ -9895,7 +9895,7 @@
         <v>285</v>
       </c>
       <c r="J128" s="4" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="K128" s="4" t="s">
         <v>443</v>
@@ -9957,7 +9957,7 @@
         <v>285</v>
       </c>
       <c r="J129" s="4" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="K129" s="4" t="s">
         <v>443</v>
@@ -10391,7 +10391,7 @@
         <v>285</v>
       </c>
       <c r="J136" s="4" t="s">
-        <v>462</v>
+        <v>285</v>
       </c>
       <c r="K136" s="4" t="s">
         <v>452</v>
@@ -10453,7 +10453,7 @@
         <v>285</v>
       </c>
       <c r="J137" s="4" t="s">
-        <v>285</v>
+        <v>462</v>
       </c>
       <c r="K137" s="4" t="s">
         <v>452</v>
@@ -10887,7 +10887,7 @@
         <v>285</v>
       </c>
       <c r="J144" s="4" t="s">
-        <v>469</v>
+        <v>285</v>
       </c>
       <c r="K144" s="4" t="s">
         <v>464</v>
@@ -10949,7 +10949,7 @@
         <v>285</v>
       </c>
       <c r="J145" s="4" t="s">
-        <v>285</v>
+        <v>469</v>
       </c>
       <c r="K145" s="4" t="s">
         <v>464</v>
@@ -11383,7 +11383,7 @@
         <v>285</v>
       </c>
       <c r="J152" s="4" t="s">
-        <v>352</v>
+        <v>285</v>
       </c>
       <c r="K152" s="4" t="s">
         <v>474</v>
@@ -11445,7 +11445,7 @@
         <v>285</v>
       </c>
       <c r="J153" s="4" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="K153" s="4" t="s">
         <v>474</v>
@@ -11879,7 +11879,7 @@
         <v>285</v>
       </c>
       <c r="J160" s="4" t="s">
-        <v>492</v>
+        <v>285</v>
       </c>
       <c r="K160" s="4" t="s">
         <v>483</v>
@@ -11941,7 +11941,7 @@
         <v>285</v>
       </c>
       <c r="J161" s="4" t="s">
-        <v>285</v>
+        <v>492</v>
       </c>
       <c r="K161" s="4" t="s">
         <v>483</v>
@@ -12375,7 +12375,7 @@
         <v>285</v>
       </c>
       <c r="J168" s="4" t="s">
-        <v>331</v>
+        <v>285</v>
       </c>
       <c r="K168" s="4" t="s">
         <v>494</v>
@@ -12437,7 +12437,7 @@
         <v>285</v>
       </c>
       <c r="J169" s="4" t="s">
-        <v>285</v>
+        <v>331</v>
       </c>
       <c r="K169" s="4" t="s">
         <v>494</v>
@@ -12871,7 +12871,7 @@
         <v>285</v>
       </c>
       <c r="J176" s="4" t="s">
-        <v>352</v>
+        <v>285</v>
       </c>
       <c r="K176" s="4" t="s">
         <v>502</v>
@@ -12933,7 +12933,7 @@
         <v>285</v>
       </c>
       <c r="J177" s="4" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="K177" s="4" t="s">
         <v>502</v>
@@ -13367,7 +13367,7 @@
         <v>285</v>
       </c>
       <c r="J184" s="4" t="s">
-        <v>520</v>
+        <v>285</v>
       </c>
       <c r="K184" s="4" t="s">
         <v>510</v>
@@ -13429,7 +13429,7 @@
         <v>285</v>
       </c>
       <c r="J185" s="4" t="s">
-        <v>285</v>
+        <v>520</v>
       </c>
       <c r="K185" s="4" t="s">
         <v>510</v>
@@ -13863,7 +13863,7 @@
         <v>285</v>
       </c>
       <c r="J192" s="4" t="s">
-        <v>526</v>
+        <v>285</v>
       </c>
       <c r="K192" s="4" t="s">
         <v>522</v>
@@ -13925,7 +13925,7 @@
         <v>285</v>
       </c>
       <c r="J193" s="4" t="s">
-        <v>285</v>
+        <v>526</v>
       </c>
       <c r="K193" s="4" t="s">
         <v>522</v>

</xml_diff>